<commit_message>
karatsuba improved and new statistics metadata collected
</commit_message>
<xml_diff>
--- a/dati karatsuba.xlsx
+++ b/dati karatsuba.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrea\Source\Repos\BigIntChallenge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EE1E5143-10D0-4966-9A47-12EAC68A4D99}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E6A840B-2874-4CA0-80CC-37B863E39D45}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="4" xr2:uid="{1987C9B5-F123-4648-B2AB-140216E6BADF}"/>
+    <workbookView minimized="1" xWindow="10710" yWindow="5265" windowWidth="10125" windowHeight="12135" activeTab="3" xr2:uid="{1987C9B5-F123-4648-B2AB-140216E6BADF}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio11" sheetId="12" r:id="rId1"/>
@@ -24,7 +24,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="34" r:id="rId6"/>
+    <pivotCache cacheId="0" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -409,46 +409,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>2.7999999999999999E-6</c:v>
+                  <c:v>1.3999999999999998E-7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.9000000000000006E-6</c:v>
+                  <c:v>3.9500000000000003E-7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.87E-5</c:v>
+                  <c:v>1.435E-6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.167E-4</c:v>
+                  <c:v>5.835E-6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.4870000000000001E-4</c:v>
+                  <c:v>2.2435000000000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.7912E-3</c:v>
+                  <c:v>8.9560000000000003E-5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.1858E-3</c:v>
+                  <c:v>3.5929000000000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.0157199999999999E-2</c:v>
+                  <c:v>1.50786E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.1171287</c:v>
+                  <c:v>5.8564350000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.45699679999999998</c:v>
+                  <c:v>2.284984E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.825566</c:v>
+                  <c:v>9.1278300000000007E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>7.2901639999999999</c:v>
+                  <c:v>0.3645082</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>29.203050000000001</c:v>
+                  <c:v>1.4601525</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>117.3004</c:v>
+                  <c:v>5.8650199999999995</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -556,46 +556,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>3.7000000000000002E-6</c:v>
+                  <c:v>1.85E-7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.13E-5</c:v>
+                  <c:v>5.6499999999999999E-7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.0099999999999998E-5</c:v>
+                  <c:v>2.5049999999999997E-6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.4909999999999999E-4</c:v>
+                  <c:v>7.4549999999999998E-6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.639E-4</c:v>
+                  <c:v>2.3195000000000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.2761999999999999E-3</c:v>
+                  <c:v>6.3810000000000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.8587999999999999E-3</c:v>
+                  <c:v>1.9294000000000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.1262899999999999E-2</c:v>
+                  <c:v>5.6314499999999992E-4</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.6338799999999997E-2</c:v>
+                  <c:v>1.81694E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.1016634</c:v>
+                  <c:v>5.0831699999999997E-3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.30568020000000001</c:v>
+                  <c:v>1.5284010000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.91939859999999995</c:v>
+                  <c:v>4.5969929999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.745584</c:v>
+                  <c:v>0.13727919999999999</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>8.2324210000000004</c:v>
+                  <c:v>0.41162105000000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -734,46 +734,46 @@
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="14"/>
                       <c:pt idx="0">
-                        <c:v>3.0000000000000001E-6</c:v>
+                        <c:v>1.4999999999999999E-7</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>9.5999999999999996E-6</c:v>
+                        <c:v>4.7999999999999996E-7</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>3.3599999999999997E-5</c:v>
+                        <c:v>1.6799999999999998E-6</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>1.395E-4</c:v>
+                        <c:v>6.9750000000000001E-6</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>5.3529999999999995E-4</c:v>
+                        <c:v>2.6764999999999999E-5</c:v>
                       </c:pt>
                       <c:pt idx="5">
-                        <c:v>2.1462E-3</c:v>
+                        <c:v>1.0731E-4</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>8.5710999999999999E-3</c:v>
+                        <c:v>4.2855500000000001E-4</c:v>
                       </c:pt>
                       <c:pt idx="7">
-                        <c:v>3.5396799999999999E-2</c:v>
+                        <c:v>1.76984E-3</c:v>
                       </c:pt>
                       <c:pt idx="8">
-                        <c:v>0.13748840000000001</c:v>
+                        <c:v>6.8744200000000009E-3</c:v>
                       </c:pt>
                       <c:pt idx="9">
-                        <c:v>0.55144230000000005</c:v>
+                        <c:v>2.7572115000000001E-2</c:v>
                       </c:pt>
                       <c:pt idx="10">
-                        <c:v>2.2009599999999998</c:v>
+                        <c:v>0.11004799999999999</c:v>
                       </c:pt>
                       <c:pt idx="11">
-                        <c:v>8.7965780000000002</c:v>
+                        <c:v>0.43982890000000002</c:v>
                       </c:pt>
                       <c:pt idx="12">
-                        <c:v>35.341760000000001</c:v>
+                        <c:v>1.767088</c:v>
                       </c:pt>
                       <c:pt idx="13">
-                        <c:v>141.70859999999999</c:v>
+                        <c:v>7.0854299999999997</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -792,7 +792,7 @@
                 <c:order val="2"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Foglio12!$D$1</c15:sqref>
@@ -833,7 +833,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Foglio12!$A$2:$A$15</c15:sqref>
@@ -890,7 +890,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Foglio12!$D$2:$D$15</c15:sqref>
@@ -901,52 +901,52 @@
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="14"/>
                       <c:pt idx="0">
-                        <c:v>3.8E-6</c:v>
+                        <c:v>1.9000000000000001E-7</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>1.11E-5</c:v>
+                        <c:v>5.5499999999999998E-7</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>5.7599999999999997E-5</c:v>
+                        <c:v>2.88E-6</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>1.5750000000000001E-4</c:v>
+                        <c:v>7.875E-6</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>4.5310000000000001E-4</c:v>
+                        <c:v>2.2654999999999999E-5</c:v>
                       </c:pt>
                       <c:pt idx="5">
-                        <c:v>1.2597999999999999E-3</c:v>
+                        <c:v>6.2989999999999992E-5</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>3.7582000000000002E-3</c:v>
+                        <c:v>1.8791000000000001E-4</c:v>
                       </c:pt>
                       <c:pt idx="7">
-                        <c:v>1.1424399999999999E-2</c:v>
+                        <c:v>5.7122E-4</c:v>
                       </c:pt>
                       <c:pt idx="8">
-                        <c:v>3.3889299999999997E-2</c:v>
+                        <c:v>1.6944649999999998E-3</c:v>
                       </c:pt>
                       <c:pt idx="9">
-                        <c:v>0.1019077</c:v>
+                        <c:v>5.095385E-3</c:v>
                       </c:pt>
                       <c:pt idx="10">
-                        <c:v>0.3051451</c:v>
+                        <c:v>1.5257255000000001E-2</c:v>
                       </c:pt>
                       <c:pt idx="11">
-                        <c:v>0.91872699999999996</c:v>
+                        <c:v>4.5936350000000001E-2</c:v>
                       </c:pt>
                       <c:pt idx="12">
-                        <c:v>2.7443149999999998</c:v>
+                        <c:v>0.13721575</c:v>
                       </c:pt>
                       <c:pt idx="13">
-                        <c:v>8.2220329999999997</c:v>
+                        <c:v>0.41110164999999999</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="1"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000002-6752-40DC-B9E3-932AD34372AE}"/>
                   </c:ext>
@@ -959,7 +959,7 @@
                 <c:order val="4"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Foglio12!$F$1</c15:sqref>
@@ -1000,7 +1000,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Foglio12!$A$2:$A$15</c15:sqref>
@@ -1057,7 +1057,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Foglio12!$F$2:$F$15</c15:sqref>
@@ -1068,52 +1068,52 @@
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="14"/>
                       <c:pt idx="0">
-                        <c:v>3.5999999999999998E-6</c:v>
+                        <c:v>1.8E-7</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>1.15E-5</c:v>
+                        <c:v>5.75E-7</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>3.8800000000000001E-5</c:v>
+                        <c:v>1.9400000000000001E-6</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>1.4420000000000001E-4</c:v>
+                        <c:v>7.2100000000000004E-6</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>4.2349999999999999E-4</c:v>
+                        <c:v>2.1175E-5</c:v>
                       </c:pt>
                       <c:pt idx="5">
-                        <c:v>1.2727999999999999E-3</c:v>
+                        <c:v>6.3639999999999994E-5</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>3.8563999999999998E-3</c:v>
+                        <c:v>1.9281999999999999E-4</c:v>
                       </c:pt>
                       <c:pt idx="7">
-                        <c:v>1.1731999999999999E-2</c:v>
+                        <c:v>5.8659999999999995E-4</c:v>
                       </c:pt>
                       <c:pt idx="8">
-                        <c:v>3.5021099999999999E-2</c:v>
+                        <c:v>1.7510550000000001E-3</c:v>
                       </c:pt>
                       <c:pt idx="9">
-                        <c:v>0.1053071</c:v>
+                        <c:v>5.2653550000000002E-3</c:v>
                       </c:pt>
                       <c:pt idx="10">
-                        <c:v>0.31508330000000001</c:v>
+                        <c:v>1.5754165000000001E-2</c:v>
                       </c:pt>
                       <c:pt idx="11">
-                        <c:v>0.94781199999999999</c:v>
+                        <c:v>4.7390599999999998E-2</c:v>
                       </c:pt>
                       <c:pt idx="12">
-                        <c:v>2.8524500000000002</c:v>
+                        <c:v>0.14262250000000001</c:v>
                       </c:pt>
                       <c:pt idx="13">
-                        <c:v>8.5020209999999992</c:v>
+                        <c:v>0.42510104999999998</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="1"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000004-6752-40DC-B9E3-932AD34372AE}"/>
                   </c:ext>
@@ -1126,7 +1126,7 @@
                 <c:order val="5"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Foglio12!$G$1</c15:sqref>
@@ -1167,7 +1167,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Foglio12!$A$2:$A$15</c15:sqref>
@@ -1224,7 +1224,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Foglio12!$G$2:$G$15</c15:sqref>
@@ -1235,52 +1235,52 @@
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="14"/>
                       <c:pt idx="0">
-                        <c:v>3.7000000000000002E-6</c:v>
+                        <c:v>1.85E-7</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>1.11E-5</c:v>
+                        <c:v>5.5499999999999998E-7</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>3.9799999999999998E-5</c:v>
+                        <c:v>1.99E-6</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>1.4300000000000001E-4</c:v>
+                        <c:v>7.1500000000000002E-6</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>4.2299999999999998E-4</c:v>
+                        <c:v>2.1149999999999999E-5</c:v>
                       </c:pt>
                       <c:pt idx="5">
-                        <c:v>1.3151E-3</c:v>
+                        <c:v>6.5754999999999996E-5</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>3.8999E-3</c:v>
+                        <c:v>1.94995E-4</c:v>
                       </c:pt>
                       <c:pt idx="7">
-                        <c:v>1.18943E-2</c:v>
+                        <c:v>5.94715E-4</c:v>
                       </c:pt>
                       <c:pt idx="8">
-                        <c:v>3.4926800000000001E-2</c:v>
+                        <c:v>1.7463400000000001E-3</c:v>
                       </c:pt>
                       <c:pt idx="9">
-                        <c:v>0.1057413</c:v>
+                        <c:v>5.2870649999999996E-3</c:v>
                       </c:pt>
                       <c:pt idx="10">
-                        <c:v>0.31829590000000002</c:v>
+                        <c:v>1.5914795000000002E-2</c:v>
                       </c:pt>
                       <c:pt idx="11">
-                        <c:v>0.95850789999999997</c:v>
+                        <c:v>4.7925394999999996E-2</c:v>
                       </c:pt>
                       <c:pt idx="12">
-                        <c:v>2.8552729999999999</c:v>
+                        <c:v>0.14276364999999999</c:v>
                       </c:pt>
                       <c:pt idx="13">
-                        <c:v>8.572419</c:v>
+                        <c:v>0.42862095</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="1"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000005-6752-40DC-B9E3-932AD34372AE}"/>
                   </c:ext>
@@ -1293,7 +1293,7 @@
                 <c:order val="6"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Foglio12!$H$1</c15:sqref>
@@ -1340,7 +1340,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Foglio12!$A$2:$A$15</c15:sqref>
@@ -1397,7 +1397,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Foglio12!$H$2:$H$15</c15:sqref>
@@ -1408,52 +1408,52 @@
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="14"/>
                       <c:pt idx="0">
-                        <c:v>3.7000000000000002E-6</c:v>
+                        <c:v>1.85E-7</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>1.7099999999999999E-5</c:v>
+                        <c:v>8.5499999999999997E-7</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>6.5599999999999995E-5</c:v>
+                        <c:v>3.2799999999999999E-6</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>1.7560000000000001E-4</c:v>
+                        <c:v>8.7800000000000006E-6</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>5.1230000000000004E-4</c:v>
+                        <c:v>2.5615000000000001E-5</c:v>
                       </c:pt>
                       <c:pt idx="5">
-                        <c:v>1.5192000000000001E-3</c:v>
+                        <c:v>7.5959999999999998E-5</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>4.6927000000000002E-3</c:v>
+                        <c:v>2.3463500000000002E-4</c:v>
                       </c:pt>
                       <c:pt idx="7">
-                        <c:v>1.34682E-2</c:v>
+                        <c:v>6.7340999999999994E-4</c:v>
                       </c:pt>
                       <c:pt idx="8">
-                        <c:v>3.9289999999999999E-2</c:v>
+                        <c:v>1.9645000000000001E-3</c:v>
                       </c:pt>
                       <c:pt idx="9">
-                        <c:v>0.1188577</c:v>
+                        <c:v>5.9428850000000002E-3</c:v>
                       </c:pt>
                       <c:pt idx="10">
-                        <c:v>0.35722219999999999</c:v>
+                        <c:v>1.7861109999999999E-2</c:v>
                       </c:pt>
                       <c:pt idx="11">
-                        <c:v>1.0784910000000001</c:v>
+                        <c:v>5.3924550000000002E-2</c:v>
                       </c:pt>
                       <c:pt idx="12">
-                        <c:v>3.2232400000000001</c:v>
+                        <c:v>0.161162</c:v>
                       </c:pt>
                       <c:pt idx="13">
-                        <c:v>9.6289660000000001</c:v>
+                        <c:v>0.4814483</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="1"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000006-6752-40DC-B9E3-932AD34372AE}"/>
                   </c:ext>
@@ -1466,7 +1466,7 @@
                 <c:order val="7"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Foglio12!$I$1</c15:sqref>
@@ -1513,7 +1513,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Foglio12!$A$2:$A$15</c15:sqref>
@@ -1570,7 +1570,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Foglio12!$I$2:$I$15</c15:sqref>
@@ -1581,52 +1581,52 @@
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="14"/>
                       <c:pt idx="0">
-                        <c:v>3.7000000000000002E-6</c:v>
+                        <c:v>1.85E-7</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>1.1E-5</c:v>
+                        <c:v>5.5000000000000003E-7</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>3.8899999999999997E-5</c:v>
+                        <c:v>1.945E-6</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>1.5770000000000001E-4</c:v>
+                        <c:v>7.8849999999999999E-6</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>6.6929999999999995E-4</c:v>
+                        <c:v>3.3464999999999999E-5</c:v>
                       </c:pt>
                       <c:pt idx="5">
-                        <c:v>2.5098E-3</c:v>
+                        <c:v>1.2548999999999999E-4</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>9.8913999999999998E-3</c:v>
+                        <c:v>4.9456999999999995E-4</c:v>
                       </c:pt>
                       <c:pt idx="7">
-                        <c:v>3.9092099999999998E-2</c:v>
+                        <c:v>1.9546049999999999E-3</c:v>
                       </c:pt>
                       <c:pt idx="8">
-                        <c:v>0.15505920000000001</c:v>
+                        <c:v>7.7529600000000006E-3</c:v>
                       </c:pt>
                       <c:pt idx="9">
-                        <c:v>0.63428430000000002</c:v>
+                        <c:v>3.1714215000000004E-2</c:v>
                       </c:pt>
                       <c:pt idx="10">
-                        <c:v>2.478062</c:v>
+                        <c:v>0.1239031</c:v>
                       </c:pt>
                       <c:pt idx="11">
-                        <c:v>9.9001459999999994</c:v>
+                        <c:v>0.49500729999999998</c:v>
                       </c:pt>
                       <c:pt idx="12">
-                        <c:v>39.630429999999997</c:v>
+                        <c:v>1.9815214999999999</c:v>
                       </c:pt>
                       <c:pt idx="13">
-                        <c:v>159.2587</c:v>
+                        <c:v>7.9629349999999999</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="1"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000007-6752-40DC-B9E3-932AD34372AE}"/>
                   </c:ext>
@@ -2054,46 +2054,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>2.7999999999999999E-6</c:v>
+                  <c:v>1.3999999999999998E-7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.9000000000000006E-6</c:v>
+                  <c:v>3.9500000000000003E-7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.87E-5</c:v>
+                  <c:v>1.435E-6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.167E-4</c:v>
+                  <c:v>5.835E-6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.4870000000000001E-4</c:v>
+                  <c:v>2.2435000000000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.7912E-3</c:v>
+                  <c:v>8.9560000000000003E-5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.1858E-3</c:v>
+                  <c:v>3.5929000000000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.0157199999999999E-2</c:v>
+                  <c:v>1.50786E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.1171287</c:v>
+                  <c:v>5.8564350000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.45699679999999998</c:v>
+                  <c:v>2.284984E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.825566</c:v>
+                  <c:v>9.1278300000000007E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>7.2901639999999999</c:v>
+                  <c:v>0.3645082</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>29.203050000000001</c:v>
+                  <c:v>1.4601525</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>117.3004</c:v>
+                  <c:v>5.8650199999999995</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2245,46 +2245,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>3.7000000000000002E-6</c:v>
+                  <c:v>1.85E-7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.13E-5</c:v>
+                  <c:v>5.6499999999999999E-7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.0099999999999998E-5</c:v>
+                  <c:v>2.5049999999999997E-6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.4909999999999999E-4</c:v>
+                  <c:v>7.4549999999999998E-6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.639E-4</c:v>
+                  <c:v>2.3195000000000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.2761999999999999E-3</c:v>
+                  <c:v>6.3810000000000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.8587999999999999E-3</c:v>
+                  <c:v>1.9294000000000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.1262899999999999E-2</c:v>
+                  <c:v>5.6314499999999992E-4</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.6338799999999997E-2</c:v>
+                  <c:v>1.81694E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.1016634</c:v>
+                  <c:v>5.0831699999999997E-3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.30568020000000001</c:v>
+                  <c:v>1.5284010000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.91939859999999995</c:v>
+                  <c:v>4.5969929999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.745584</c:v>
+                  <c:v>0.13727919999999999</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>8.2324210000000004</c:v>
+                  <c:v>0.41162105000000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2423,46 +2423,46 @@
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="14"/>
                       <c:pt idx="0">
-                        <c:v>3.0000000000000001E-6</c:v>
+                        <c:v>1.4999999999999999E-7</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>9.5999999999999996E-6</c:v>
+                        <c:v>4.7999999999999996E-7</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>3.3599999999999997E-5</c:v>
+                        <c:v>1.6799999999999998E-6</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>1.395E-4</c:v>
+                        <c:v>6.9750000000000001E-6</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>5.3529999999999995E-4</c:v>
+                        <c:v>2.6764999999999999E-5</c:v>
                       </c:pt>
                       <c:pt idx="5">
-                        <c:v>2.1462E-3</c:v>
+                        <c:v>1.0731E-4</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>8.5710999999999999E-3</c:v>
+                        <c:v>4.2855500000000001E-4</c:v>
                       </c:pt>
                       <c:pt idx="7">
-                        <c:v>3.5396799999999999E-2</c:v>
+                        <c:v>1.76984E-3</c:v>
                       </c:pt>
                       <c:pt idx="8">
-                        <c:v>0.13748840000000001</c:v>
+                        <c:v>6.8744200000000009E-3</c:v>
                       </c:pt>
                       <c:pt idx="9">
-                        <c:v>0.55144230000000005</c:v>
+                        <c:v>2.7572115000000001E-2</c:v>
                       </c:pt>
                       <c:pt idx="10">
-                        <c:v>2.2009599999999998</c:v>
+                        <c:v>0.11004799999999999</c:v>
                       </c:pt>
                       <c:pt idx="11">
-                        <c:v>8.7965780000000002</c:v>
+                        <c:v>0.43982890000000002</c:v>
                       </c:pt>
                       <c:pt idx="12">
-                        <c:v>35.341760000000001</c:v>
+                        <c:v>1.767088</c:v>
                       </c:pt>
                       <c:pt idx="13">
-                        <c:v>141.70859999999999</c:v>
+                        <c:v>7.0854299999999997</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2590,52 +2590,52 @@
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="14"/>
                       <c:pt idx="0">
-                        <c:v>3.8E-6</c:v>
+                        <c:v>1.9000000000000001E-7</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>1.11E-5</c:v>
+                        <c:v>5.5499999999999998E-7</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>5.7599999999999997E-5</c:v>
+                        <c:v>2.88E-6</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>1.5750000000000001E-4</c:v>
+                        <c:v>7.875E-6</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>4.5310000000000001E-4</c:v>
+                        <c:v>2.2654999999999999E-5</c:v>
                       </c:pt>
                       <c:pt idx="5">
-                        <c:v>1.2597999999999999E-3</c:v>
+                        <c:v>6.2989999999999992E-5</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>3.7582000000000002E-3</c:v>
+                        <c:v>1.8791000000000001E-4</c:v>
                       </c:pt>
                       <c:pt idx="7">
-                        <c:v>1.1424399999999999E-2</c:v>
+                        <c:v>5.7122E-4</c:v>
                       </c:pt>
                       <c:pt idx="8">
-                        <c:v>3.3889299999999997E-2</c:v>
+                        <c:v>1.6944649999999998E-3</c:v>
                       </c:pt>
                       <c:pt idx="9">
-                        <c:v>0.1019077</c:v>
+                        <c:v>5.095385E-3</c:v>
                       </c:pt>
                       <c:pt idx="10">
-                        <c:v>0.3051451</c:v>
+                        <c:v>1.5257255000000001E-2</c:v>
                       </c:pt>
                       <c:pt idx="11">
-                        <c:v>0.91872699999999996</c:v>
+                        <c:v>4.5936350000000001E-2</c:v>
                       </c:pt>
                       <c:pt idx="12">
-                        <c:v>2.7443149999999998</c:v>
+                        <c:v>0.13721575</c:v>
                       </c:pt>
                       <c:pt idx="13">
-                        <c:v>8.2220329999999997</c:v>
+                        <c:v>0.41110164999999999</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="1"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000003-0F84-4A53-8C29-09BD19314633}"/>
                   </c:ext>
@@ -2757,52 +2757,52 @@
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="14"/>
                       <c:pt idx="0">
-                        <c:v>3.5999999999999998E-6</c:v>
+                        <c:v>1.8E-7</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>1.15E-5</c:v>
+                        <c:v>5.75E-7</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>3.8800000000000001E-5</c:v>
+                        <c:v>1.9400000000000001E-6</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>1.4420000000000001E-4</c:v>
+                        <c:v>7.2100000000000004E-6</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>4.2349999999999999E-4</c:v>
+                        <c:v>2.1175E-5</c:v>
                       </c:pt>
                       <c:pt idx="5">
-                        <c:v>1.2727999999999999E-3</c:v>
+                        <c:v>6.3639999999999994E-5</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>3.8563999999999998E-3</c:v>
+                        <c:v>1.9281999999999999E-4</c:v>
                       </c:pt>
                       <c:pt idx="7">
-                        <c:v>1.1731999999999999E-2</c:v>
+                        <c:v>5.8659999999999995E-4</c:v>
                       </c:pt>
                       <c:pt idx="8">
-                        <c:v>3.5021099999999999E-2</c:v>
+                        <c:v>1.7510550000000001E-3</c:v>
                       </c:pt>
                       <c:pt idx="9">
-                        <c:v>0.1053071</c:v>
+                        <c:v>5.2653550000000002E-3</c:v>
                       </c:pt>
                       <c:pt idx="10">
-                        <c:v>0.31508330000000001</c:v>
+                        <c:v>1.5754165000000001E-2</c:v>
                       </c:pt>
                       <c:pt idx="11">
-                        <c:v>0.94781199999999999</c:v>
+                        <c:v>4.7390599999999998E-2</c:v>
                       </c:pt>
                       <c:pt idx="12">
-                        <c:v>2.8524500000000002</c:v>
+                        <c:v>0.14262250000000001</c:v>
                       </c:pt>
                       <c:pt idx="13">
-                        <c:v>8.5020209999999992</c:v>
+                        <c:v>0.42510104999999998</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="1"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000004-0F84-4A53-8C29-09BD19314633}"/>
                   </c:ext>
@@ -2924,52 +2924,52 @@
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="14"/>
                       <c:pt idx="0">
-                        <c:v>3.7000000000000002E-6</c:v>
+                        <c:v>1.85E-7</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>1.11E-5</c:v>
+                        <c:v>5.5499999999999998E-7</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>3.9799999999999998E-5</c:v>
+                        <c:v>1.99E-6</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>1.4300000000000001E-4</c:v>
+                        <c:v>7.1500000000000002E-6</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>4.2299999999999998E-4</c:v>
+                        <c:v>2.1149999999999999E-5</c:v>
                       </c:pt>
                       <c:pt idx="5">
-                        <c:v>1.3151E-3</c:v>
+                        <c:v>6.5754999999999996E-5</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>3.8999E-3</c:v>
+                        <c:v>1.94995E-4</c:v>
                       </c:pt>
                       <c:pt idx="7">
-                        <c:v>1.18943E-2</c:v>
+                        <c:v>5.94715E-4</c:v>
                       </c:pt>
                       <c:pt idx="8">
-                        <c:v>3.4926800000000001E-2</c:v>
+                        <c:v>1.7463400000000001E-3</c:v>
                       </c:pt>
                       <c:pt idx="9">
-                        <c:v>0.1057413</c:v>
+                        <c:v>5.2870649999999996E-3</c:v>
                       </c:pt>
                       <c:pt idx="10">
-                        <c:v>0.31829590000000002</c:v>
+                        <c:v>1.5914795000000002E-2</c:v>
                       </c:pt>
                       <c:pt idx="11">
-                        <c:v>0.95850789999999997</c:v>
+                        <c:v>4.7925394999999996E-2</c:v>
                       </c:pt>
                       <c:pt idx="12">
-                        <c:v>2.8552729999999999</c:v>
+                        <c:v>0.14276364999999999</c:v>
                       </c:pt>
                       <c:pt idx="13">
-                        <c:v>8.572419</c:v>
+                        <c:v>0.42862095</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="1"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000005-0F84-4A53-8C29-09BD19314633}"/>
                   </c:ext>
@@ -3097,52 +3097,52 @@
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="14"/>
                       <c:pt idx="0">
-                        <c:v>3.7000000000000002E-6</c:v>
+                        <c:v>1.85E-7</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>1.7099999999999999E-5</c:v>
+                        <c:v>8.5499999999999997E-7</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>6.5599999999999995E-5</c:v>
+                        <c:v>3.2799999999999999E-6</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>1.7560000000000001E-4</c:v>
+                        <c:v>8.7800000000000006E-6</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>5.1230000000000004E-4</c:v>
+                        <c:v>2.5615000000000001E-5</c:v>
                       </c:pt>
                       <c:pt idx="5">
-                        <c:v>1.5192000000000001E-3</c:v>
+                        <c:v>7.5959999999999998E-5</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>4.6927000000000002E-3</c:v>
+                        <c:v>2.3463500000000002E-4</c:v>
                       </c:pt>
                       <c:pt idx="7">
-                        <c:v>1.34682E-2</c:v>
+                        <c:v>6.7340999999999994E-4</c:v>
                       </c:pt>
                       <c:pt idx="8">
-                        <c:v>3.9289999999999999E-2</c:v>
+                        <c:v>1.9645000000000001E-3</c:v>
                       </c:pt>
                       <c:pt idx="9">
-                        <c:v>0.1188577</c:v>
+                        <c:v>5.9428850000000002E-3</c:v>
                       </c:pt>
                       <c:pt idx="10">
-                        <c:v>0.35722219999999999</c:v>
+                        <c:v>1.7861109999999999E-2</c:v>
                       </c:pt>
                       <c:pt idx="11">
-                        <c:v>1.0784910000000001</c:v>
+                        <c:v>5.3924550000000002E-2</c:v>
                       </c:pt>
                       <c:pt idx="12">
-                        <c:v>3.2232400000000001</c:v>
+                        <c:v>0.161162</c:v>
                       </c:pt>
                       <c:pt idx="13">
-                        <c:v>9.6289660000000001</c:v>
+                        <c:v>0.4814483</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="1"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000006-0F84-4A53-8C29-09BD19314633}"/>
                   </c:ext>
@@ -3270,52 +3270,52 @@
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="14"/>
                       <c:pt idx="0">
-                        <c:v>3.7000000000000002E-6</c:v>
+                        <c:v>1.85E-7</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>1.1E-5</c:v>
+                        <c:v>5.5000000000000003E-7</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>3.8899999999999997E-5</c:v>
+                        <c:v>1.945E-6</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>1.5770000000000001E-4</c:v>
+                        <c:v>7.8849999999999999E-6</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>6.6929999999999995E-4</c:v>
+                        <c:v>3.3464999999999999E-5</c:v>
                       </c:pt>
                       <c:pt idx="5">
-                        <c:v>2.5098E-3</c:v>
+                        <c:v>1.2548999999999999E-4</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>9.8913999999999998E-3</c:v>
+                        <c:v>4.9456999999999995E-4</c:v>
                       </c:pt>
                       <c:pt idx="7">
-                        <c:v>3.9092099999999998E-2</c:v>
+                        <c:v>1.9546049999999999E-3</c:v>
                       </c:pt>
                       <c:pt idx="8">
-                        <c:v>0.15505920000000001</c:v>
+                        <c:v>7.7529600000000006E-3</c:v>
                       </c:pt>
                       <c:pt idx="9">
-                        <c:v>0.63428430000000002</c:v>
+                        <c:v>3.1714215000000004E-2</c:v>
                       </c:pt>
                       <c:pt idx="10">
-                        <c:v>2.478062</c:v>
+                        <c:v>0.1239031</c:v>
                       </c:pt>
                       <c:pt idx="11">
-                        <c:v>9.9001459999999994</c:v>
+                        <c:v>0.49500729999999998</c:v>
                       </c:pt>
                       <c:pt idx="12">
-                        <c:v>39.630429999999997</c:v>
+                        <c:v>1.9815214999999999</c:v>
                       </c:pt>
                       <c:pt idx="13">
-                        <c:v>159.2587</c:v>
+                        <c:v>7.9629349999999999</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="1"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000007-0F84-4A53-8C29-09BD19314633}"/>
                   </c:ext>
@@ -4658,7 +4658,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{78598AE9-647A-481C-B788-8A3ECDE20D85}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="115" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="115" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4669,7 +4669,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{2C09EAD8-8A82-4ADD-A062-E33334D56D8C}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" workbookViewId="0"/>
+    <sheetView zoomScale="115" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4680,7 +4680,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9298867" cy="6078183"/>
+    <xdr:ext cx="9301370" cy="6071152"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Grafico 1">
@@ -4713,7 +4713,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9298867" cy="6078183"/>
+    <xdr:ext cx="9301370" cy="6071152"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Grafico 1">
@@ -6910,7 +6910,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4A577AE7-3653-469E-ABB4-55BDDA708FCC}" name="Tabella pivot7" cacheId="34" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4A577AE7-3653-469E-ABB4-55BDDA708FCC}" name="Tabella pivot7" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:J19" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="11">
     <pivotField axis="axisCol" showAll="0">
@@ -13626,7 +13626,7 @@
   <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:I15"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13672,409 +13672,414 @@
       <c r="A2" s="4">
         <v>4</v>
       </c>
-      <c r="B2" s="1">
-        <v>3.0000000000000001E-6</v>
-      </c>
-      <c r="C2" s="1">
-        <v>2.7999999999999999E-6</v>
-      </c>
-      <c r="D2" s="1">
-        <v>3.8E-6</v>
-      </c>
-      <c r="E2" s="1">
-        <v>3.7000000000000002E-6</v>
-      </c>
-      <c r="F2" s="1">
-        <v>3.5999999999999998E-6</v>
-      </c>
-      <c r="G2" s="1">
-        <v>3.7000000000000002E-6</v>
-      </c>
-      <c r="H2" s="1">
-        <v>3.7000000000000002E-6</v>
-      </c>
-      <c r="I2" s="1">
-        <v>3.7000000000000002E-6</v>
+      <c r="B2">
+        <v>1.4999999999999999E-7</v>
+      </c>
+      <c r="C2">
+        <v>1.3999999999999998E-7</v>
+      </c>
+      <c r="D2">
+        <v>1.9000000000000001E-7</v>
+      </c>
+      <c r="E2">
+        <v>1.85E-7</v>
+      </c>
+      <c r="F2">
+        <v>1.8E-7</v>
+      </c>
+      <c r="G2">
+        <v>1.85E-7</v>
+      </c>
+      <c r="H2">
+        <v>1.85E-7</v>
+      </c>
+      <c r="I2">
+        <v>1.85E-7</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>8</v>
       </c>
-      <c r="B3" s="1">
-        <v>9.5999999999999996E-6</v>
-      </c>
-      <c r="C3" s="1">
-        <v>7.9000000000000006E-6</v>
-      </c>
-      <c r="D3" s="1">
-        <v>1.11E-5</v>
-      </c>
-      <c r="E3" s="1">
-        <v>1.13E-5</v>
-      </c>
-      <c r="F3" s="1">
-        <v>1.15E-5</v>
-      </c>
-      <c r="G3" s="1">
-        <v>1.11E-5</v>
-      </c>
-      <c r="H3" s="1">
-        <v>1.7099999999999999E-5</v>
-      </c>
-      <c r="I3" s="1">
-        <v>1.1E-5</v>
+      <c r="B3">
+        <v>4.7999999999999996E-7</v>
+      </c>
+      <c r="C3">
+        <v>3.9500000000000003E-7</v>
+      </c>
+      <c r="D3">
+        <v>5.5499999999999998E-7</v>
+      </c>
+      <c r="E3">
+        <v>5.6499999999999999E-7</v>
+      </c>
+      <c r="F3">
+        <v>5.75E-7</v>
+      </c>
+      <c r="G3">
+        <v>5.5499999999999998E-7</v>
+      </c>
+      <c r="H3">
+        <v>8.5499999999999997E-7</v>
+      </c>
+      <c r="I3">
+        <v>5.5000000000000003E-7</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>16</v>
       </c>
-      <c r="B4" s="1">
-        <v>3.3599999999999997E-5</v>
-      </c>
-      <c r="C4" s="1">
-        <v>2.87E-5</v>
-      </c>
-      <c r="D4" s="1">
-        <v>5.7599999999999997E-5</v>
-      </c>
-      <c r="E4" s="1">
-        <v>5.0099999999999998E-5</v>
-      </c>
-      <c r="F4" s="1">
-        <v>3.8800000000000001E-5</v>
-      </c>
-      <c r="G4" s="1">
-        <v>3.9799999999999998E-5</v>
-      </c>
-      <c r="H4" s="1">
-        <v>6.5599999999999995E-5</v>
-      </c>
-      <c r="I4" s="1">
-        <v>3.8899999999999997E-5</v>
+      <c r="B4">
+        <v>1.6799999999999998E-6</v>
+      </c>
+      <c r="C4">
+        <v>1.435E-6</v>
+      </c>
+      <c r="D4">
+        <v>2.88E-6</v>
+      </c>
+      <c r="E4">
+        <v>2.5049999999999997E-6</v>
+      </c>
+      <c r="F4">
+        <v>1.9400000000000001E-6</v>
+      </c>
+      <c r="G4">
+        <v>1.99E-6</v>
+      </c>
+      <c r="H4">
+        <v>3.2799999999999999E-6</v>
+      </c>
+      <c r="I4">
+        <v>1.945E-6</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>32</v>
       </c>
-      <c r="B5" s="1">
-        <v>1.395E-4</v>
-      </c>
-      <c r="C5" s="1">
-        <v>1.167E-4</v>
-      </c>
-      <c r="D5" s="1">
-        <v>1.5750000000000001E-4</v>
-      </c>
-      <c r="E5" s="1">
-        <v>1.4909999999999999E-4</v>
-      </c>
-      <c r="F5" s="1">
-        <v>1.4420000000000001E-4</v>
-      </c>
-      <c r="G5" s="1">
-        <v>1.4300000000000001E-4</v>
-      </c>
-      <c r="H5" s="1">
-        <v>1.7560000000000001E-4</v>
-      </c>
-      <c r="I5" s="1">
-        <v>1.5770000000000001E-4</v>
+      <c r="B5">
+        <v>6.9750000000000001E-6</v>
+      </c>
+      <c r="C5">
+        <v>5.835E-6</v>
+      </c>
+      <c r="D5">
+        <v>7.875E-6</v>
+      </c>
+      <c r="E5">
+        <v>7.4549999999999998E-6</v>
+      </c>
+      <c r="F5">
+        <v>7.2100000000000004E-6</v>
+      </c>
+      <c r="G5">
+        <v>7.1500000000000002E-6</v>
+      </c>
+      <c r="H5">
+        <v>8.7800000000000006E-6</v>
+      </c>
+      <c r="I5">
+        <v>7.8849999999999999E-6</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>64</v>
       </c>
-      <c r="B6" s="1">
-        <v>5.3529999999999995E-4</v>
-      </c>
-      <c r="C6" s="1">
-        <v>4.4870000000000001E-4</v>
-      </c>
-      <c r="D6" s="1">
-        <v>4.5310000000000001E-4</v>
-      </c>
-      <c r="E6" s="1">
-        <v>4.639E-4</v>
-      </c>
-      <c r="F6" s="1">
-        <v>4.2349999999999999E-4</v>
-      </c>
-      <c r="G6" s="1">
-        <v>4.2299999999999998E-4</v>
-      </c>
-      <c r="H6" s="1">
-        <v>5.1230000000000004E-4</v>
-      </c>
-      <c r="I6" s="1">
-        <v>6.6929999999999995E-4</v>
+      <c r="B6">
+        <v>2.6764999999999999E-5</v>
+      </c>
+      <c r="C6">
+        <v>2.2435000000000001E-5</v>
+      </c>
+      <c r="D6">
+        <v>2.2654999999999999E-5</v>
+      </c>
+      <c r="E6">
+        <v>2.3195000000000001E-5</v>
+      </c>
+      <c r="F6">
+        <v>2.1175E-5</v>
+      </c>
+      <c r="G6">
+        <v>2.1149999999999999E-5</v>
+      </c>
+      <c r="H6">
+        <v>2.5615000000000001E-5</v>
+      </c>
+      <c r="I6">
+        <v>3.3464999999999999E-5</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>128</v>
       </c>
-      <c r="B7" s="1">
-        <v>2.1462E-3</v>
-      </c>
-      <c r="C7" s="1">
-        <v>1.7912E-3</v>
-      </c>
-      <c r="D7" s="1">
-        <v>1.2597999999999999E-3</v>
-      </c>
-      <c r="E7" s="1">
-        <v>1.2761999999999999E-3</v>
-      </c>
-      <c r="F7" s="1">
-        <v>1.2727999999999999E-3</v>
-      </c>
-      <c r="G7" s="1">
-        <v>1.3151E-3</v>
-      </c>
-      <c r="H7" s="1">
-        <v>1.5192000000000001E-3</v>
-      </c>
-      <c r="I7" s="1">
-        <v>2.5098E-3</v>
+      <c r="B7">
+        <v>1.0731E-4</v>
+      </c>
+      <c r="C7">
+        <v>8.9560000000000003E-5</v>
+      </c>
+      <c r="D7">
+        <v>6.2989999999999992E-5</v>
+      </c>
+      <c r="E7">
+        <v>6.3810000000000001E-5</v>
+      </c>
+      <c r="F7">
+        <v>6.3639999999999994E-5</v>
+      </c>
+      <c r="G7">
+        <v>6.5754999999999996E-5</v>
+      </c>
+      <c r="H7">
+        <v>7.5959999999999998E-5</v>
+      </c>
+      <c r="I7">
+        <v>1.2548999999999999E-4</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>256</v>
       </c>
-      <c r="B8" s="1">
-        <v>8.5710999999999999E-3</v>
-      </c>
-      <c r="C8" s="1">
-        <v>7.1858E-3</v>
-      </c>
-      <c r="D8" s="1">
-        <v>3.7582000000000002E-3</v>
-      </c>
-      <c r="E8" s="1">
-        <v>3.8587999999999999E-3</v>
-      </c>
-      <c r="F8" s="1">
-        <v>3.8563999999999998E-3</v>
-      </c>
-      <c r="G8" s="1">
-        <v>3.8999E-3</v>
-      </c>
-      <c r="H8" s="1">
-        <v>4.6927000000000002E-3</v>
-      </c>
-      <c r="I8" s="1">
-        <v>9.8913999999999998E-3</v>
+      <c r="B8">
+        <v>4.2855500000000001E-4</v>
+      </c>
+      <c r="C8">
+        <v>3.5929000000000001E-4</v>
+      </c>
+      <c r="D8">
+        <v>1.8791000000000001E-4</v>
+      </c>
+      <c r="E8">
+        <v>1.9294000000000001E-4</v>
+      </c>
+      <c r="F8">
+        <v>1.9281999999999999E-4</v>
+      </c>
+      <c r="G8">
+        <v>1.94995E-4</v>
+      </c>
+      <c r="H8">
+        <v>2.3463500000000002E-4</v>
+      </c>
+      <c r="I8">
+        <v>4.9456999999999995E-4</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>512</v>
       </c>
-      <c r="B9" s="1">
-        <v>3.5396799999999999E-2</v>
-      </c>
-      <c r="C9" s="1">
-        <v>3.0157199999999999E-2</v>
-      </c>
-      <c r="D9" s="1">
-        <v>1.1424399999999999E-2</v>
-      </c>
-      <c r="E9" s="1">
-        <v>1.1262899999999999E-2</v>
-      </c>
-      <c r="F9" s="1">
-        <v>1.1731999999999999E-2</v>
-      </c>
-      <c r="G9" s="1">
-        <v>1.18943E-2</v>
-      </c>
-      <c r="H9" s="1">
-        <v>1.34682E-2</v>
-      </c>
-      <c r="I9" s="1">
-        <v>3.9092099999999998E-2</v>
+      <c r="B9">
+        <v>1.76984E-3</v>
+      </c>
+      <c r="C9">
+        <v>1.50786E-3</v>
+      </c>
+      <c r="D9">
+        <v>5.7122E-4</v>
+      </c>
+      <c r="E9">
+        <v>5.6314499999999992E-4</v>
+      </c>
+      <c r="F9">
+        <v>5.8659999999999995E-4</v>
+      </c>
+      <c r="G9">
+        <v>5.94715E-4</v>
+      </c>
+      <c r="H9">
+        <v>6.7340999999999994E-4</v>
+      </c>
+      <c r="I9">
+        <v>1.9546049999999999E-3</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>1024</v>
       </c>
-      <c r="B10" s="1">
-        <v>0.13748840000000001</v>
-      </c>
-      <c r="C10" s="1">
-        <v>0.1171287</v>
-      </c>
-      <c r="D10" s="1">
-        <v>3.3889299999999997E-2</v>
-      </c>
-      <c r="E10" s="1">
-        <v>3.6338799999999997E-2</v>
-      </c>
-      <c r="F10" s="1">
-        <v>3.5021099999999999E-2</v>
-      </c>
-      <c r="G10" s="1">
-        <v>3.4926800000000001E-2</v>
-      </c>
-      <c r="H10" s="1">
-        <v>3.9289999999999999E-2</v>
-      </c>
-      <c r="I10" s="1">
-        <v>0.15505920000000001</v>
+      <c r="B10">
+        <v>6.8744200000000009E-3</v>
+      </c>
+      <c r="C10">
+        <v>5.8564350000000001E-3</v>
+      </c>
+      <c r="D10">
+        <v>1.6944649999999998E-3</v>
+      </c>
+      <c r="E10">
+        <v>1.81694E-3</v>
+      </c>
+      <c r="F10">
+        <v>1.7510550000000001E-3</v>
+      </c>
+      <c r="G10">
+        <v>1.7463400000000001E-3</v>
+      </c>
+      <c r="H10">
+        <v>1.9645000000000001E-3</v>
+      </c>
+      <c r="I10">
+        <v>7.7529600000000006E-3</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>2048</v>
       </c>
-      <c r="B11" s="1">
-        <v>0.55144230000000005</v>
-      </c>
-      <c r="C11" s="1">
-        <v>0.45699679999999998</v>
-      </c>
-      <c r="D11" s="1">
-        <v>0.1019077</v>
-      </c>
-      <c r="E11" s="1">
-        <v>0.1016634</v>
-      </c>
-      <c r="F11" s="1">
-        <v>0.1053071</v>
-      </c>
-      <c r="G11" s="1">
-        <v>0.1057413</v>
-      </c>
-      <c r="H11" s="1">
-        <v>0.1188577</v>
-      </c>
-      <c r="I11" s="1">
-        <v>0.63428430000000002</v>
+      <c r="B11">
+        <v>2.7572115000000001E-2</v>
+      </c>
+      <c r="C11">
+        <v>2.284984E-2</v>
+      </c>
+      <c r="D11">
+        <v>5.095385E-3</v>
+      </c>
+      <c r="E11">
+        <v>5.0831699999999997E-3</v>
+      </c>
+      <c r="F11">
+        <v>5.2653550000000002E-3</v>
+      </c>
+      <c r="G11">
+        <v>5.2870649999999996E-3</v>
+      </c>
+      <c r="H11">
+        <v>5.9428850000000002E-3</v>
+      </c>
+      <c r="I11">
+        <v>3.1714215000000004E-2</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>4096</v>
       </c>
-      <c r="B12" s="1">
-        <v>2.2009599999999998</v>
-      </c>
-      <c r="C12" s="1">
-        <v>1.825566</v>
-      </c>
-      <c r="D12" s="1">
-        <v>0.3051451</v>
-      </c>
-      <c r="E12" s="1">
-        <v>0.30568020000000001</v>
-      </c>
-      <c r="F12" s="1">
-        <v>0.31508330000000001</v>
-      </c>
-      <c r="G12" s="1">
-        <v>0.31829590000000002</v>
-      </c>
-      <c r="H12" s="1">
-        <v>0.35722219999999999</v>
-      </c>
-      <c r="I12" s="1">
-        <v>2.478062</v>
+      <c r="B12">
+        <v>0.11004799999999999</v>
+      </c>
+      <c r="C12">
+        <v>9.1278300000000007E-2</v>
+      </c>
+      <c r="D12">
+        <v>1.5257255000000001E-2</v>
+      </c>
+      <c r="E12">
+        <v>1.5284010000000001E-2</v>
+      </c>
+      <c r="F12">
+        <v>1.5754165000000001E-2</v>
+      </c>
+      <c r="G12">
+        <v>1.5914795000000002E-2</v>
+      </c>
+      <c r="H12">
+        <v>1.7861109999999999E-2</v>
+      </c>
+      <c r="I12">
+        <v>0.1239031</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>8192</v>
       </c>
-      <c r="B13" s="1">
-        <v>8.7965780000000002</v>
-      </c>
-      <c r="C13" s="1">
-        <v>7.2901639999999999</v>
-      </c>
-      <c r="D13" s="1">
-        <v>0.91872699999999996</v>
-      </c>
-      <c r="E13" s="1">
-        <v>0.91939859999999995</v>
-      </c>
-      <c r="F13" s="1">
-        <v>0.94781199999999999</v>
-      </c>
-      <c r="G13" s="1">
-        <v>0.95850789999999997</v>
-      </c>
-      <c r="H13" s="1">
-        <v>1.0784910000000001</v>
-      </c>
-      <c r="I13" s="1">
-        <v>9.9001459999999994</v>
+      <c r="B13">
+        <v>0.43982890000000002</v>
+      </c>
+      <c r="C13">
+        <v>0.3645082</v>
+      </c>
+      <c r="D13">
+        <v>4.5936350000000001E-2</v>
+      </c>
+      <c r="E13">
+        <v>4.5969929999999999E-2</v>
+      </c>
+      <c r="F13">
+        <v>4.7390599999999998E-2</v>
+      </c>
+      <c r="G13">
+        <v>4.7925394999999996E-2</v>
+      </c>
+      <c r="H13">
+        <v>5.3924550000000002E-2</v>
+      </c>
+      <c r="I13">
+        <v>0.49500729999999998</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>16384</v>
       </c>
-      <c r="B14" s="1">
-        <v>35.341760000000001</v>
-      </c>
-      <c r="C14" s="1">
-        <v>29.203050000000001</v>
-      </c>
-      <c r="D14" s="1">
-        <v>2.7443149999999998</v>
-      </c>
-      <c r="E14" s="1">
-        <v>2.745584</v>
-      </c>
-      <c r="F14" s="1">
-        <v>2.8524500000000002</v>
-      </c>
-      <c r="G14" s="1">
-        <v>2.8552729999999999</v>
-      </c>
-      <c r="H14" s="1">
-        <v>3.2232400000000001</v>
-      </c>
-      <c r="I14" s="1">
-        <v>39.630429999999997</v>
+      <c r="B14">
+        <v>1.767088</v>
+      </c>
+      <c r="C14">
+        <v>1.4601525</v>
+      </c>
+      <c r="D14">
+        <v>0.13721575</v>
+      </c>
+      <c r="E14">
+        <v>0.13727919999999999</v>
+      </c>
+      <c r="F14">
+        <v>0.14262250000000001</v>
+      </c>
+      <c r="G14">
+        <v>0.14276364999999999</v>
+      </c>
+      <c r="H14">
+        <v>0.161162</v>
+      </c>
+      <c r="I14">
+        <v>1.9815214999999999</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>32768</v>
       </c>
-      <c r="B15" s="1">
-        <v>141.70859999999999</v>
-      </c>
-      <c r="C15" s="1">
-        <v>117.3004</v>
-      </c>
-      <c r="D15" s="1">
-        <v>8.2220329999999997</v>
-      </c>
-      <c r="E15" s="1">
-        <v>8.2324210000000004</v>
-      </c>
-      <c r="F15" s="1">
-        <v>8.5020209999999992</v>
-      </c>
-      <c r="G15" s="1">
-        <v>8.572419</v>
-      </c>
-      <c r="H15" s="1">
-        <v>9.6289660000000001</v>
-      </c>
-      <c r="I15" s="1">
-        <v>159.2587</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>7.0854299999999997</v>
+      </c>
+      <c r="C15">
+        <v>5.8650199999999995</v>
+      </c>
+      <c r="D15">
+        <v>0.41110164999999999</v>
+      </c>
+      <c r="E15">
+        <v>0.41162105000000004</v>
+      </c>
+      <c r="F15">
+        <v>0.42510104999999998</v>
+      </c>
+      <c r="G15">
+        <v>0.42862095</v>
+      </c>
+      <c r="H15">
+        <v>0.4814483</v>
+      </c>
+      <c r="I15">
+        <v>7.9629349999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E19">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>320</v>
       </c>
@@ -14091,7 +14096,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>1280</v>
       </c>
@@ -14108,7 +14113,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>5120</v>
       </c>
@@ -14125,7 +14130,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>20480</v>
       </c>
@@ -14142,7 +14147,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>81920</v>
       </c>
@@ -14159,7 +14164,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>327680</v>
       </c>
@@ -14176,7 +14181,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>1310720</v>
       </c>
@@ -14193,7 +14198,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>5242880</v>
       </c>
@@ -14210,7 +14215,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>20971520</v>
       </c>
@@ -14227,7 +14232,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>83886080</v>
       </c>
@@ -14244,7 +14249,7 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>335544300</v>
       </c>
@@ -14261,7 +14266,7 @@
         <v>4096</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>1342177000</v>
       </c>
@@ -14278,7 +14283,7 @@
         <v>8192</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>5368709000</v>
       </c>

</xml_diff>